<commit_message>
Adding data, moving processing out of the qmd, and writing a ton of stuff on repro, repeat, and algs
</commit_message>
<xml_diff>
--- a/data/Study_Summary.xlsx
+++ b/data/Study_Summary.xlsx
@@ -212,13 +212,13 @@
     <t xml:space="preserve">Ames II accuracy study writeup</t>
   </si>
   <si>
-    <t xml:space="preserve">Partially [^18]</t>
+    <t xml:space="preserve">Partially [^ames2-data]</t>
   </si>
   <si>
     <t xml:space="preserve">Unreported</t>
   </si>
   <si>
-    <t xml:space="preserve">0.356 [^19]</t>
+    <t xml:space="preserve">0.356 [^ames2-nonresponse]</t>
   </si>
   <si>
     <t xml:space="preserve">baldwinStudyExaminerAccuracy2023</t>
@@ -278,7 +278,7 @@
     <t xml:space="preserve">Virtual</t>
   </si>
   <si>
-    <t xml:space="preserve">$\geq$ 0.29 [^17]</t>
+    <t xml:space="preserve">$\geq$ 0.29 [^chapnick-dropout]</t>
   </si>
   <si>
     <t xml:space="preserve">lawEvaluatingFirearmExaminer2021</t>
@@ -353,7 +353,7 @@
     <t xml:space="preserve">Slide</t>
   </si>
   <si>
-    <t xml:space="preserve">0.23 [^16]</t>
+    <t xml:space="preserve">0.23 [^fadul-dropout]</t>
   </si>
   <si>
     <t xml:space="preserve">pauw2013faid</t>
@@ -368,7 +368,7 @@
     <t xml:space="preserve">Extractor</t>
   </si>
   <si>
-    <t xml:space="preserve">Unreported [^15]</t>
+    <t xml:space="preserve">Unreported [^mayland-partial]</t>
   </si>
   <si>
     <t xml:space="preserve">lyonsIdentificationConsecutivelyManufactured2009</t>
@@ -565,11 +565,11 @@
   <dimension ref="A1:AS27"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="15" ySplit="1" topLeftCell="W2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="15" ySplit="1" topLeftCell="P2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="W1" activeCellId="0" sqref="W1"/>
+      <selection pane="topRight" activeCell="P1" activeCellId="0" sqref="P1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AN30" activeCellId="0" sqref="AN30"/>
+      <selection pane="bottomRight" activeCell="M6" activeCellId="0" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -577,8 +577,10 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="38.7"/>
     <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="5" min="4" style="1" width="11.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="10.06"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="1" width="5.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="15.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="9.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="5.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="21.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="18.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="7.93"/>
     <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="33" min="33" style="1" width="11.53"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="35" min="34" style="2" width="11.53"/>
@@ -837,86 +839,86 @@
       <c r="A3" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="B3" s="1" t="n">
         <v>2024</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="F3" s="0" t="s">
+      <c r="F3" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="G3" s="0" t="s">
+      <c r="G3" s="1" t="s">
         <v>46</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>47</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="K3" s="0" t="s">
+      <c r="K3" s="1" t="s">
         <v>49</v>
       </c>
       <c r="L3" s="1" t="n">
         <f aca="false">28/(49+28)</f>
         <v>0.363636363636364</v>
       </c>
-      <c r="M3" s="0" t="n">
+      <c r="M3" s="1" t="n">
         <f aca="false">1-(1443+1441)/(49*90)</f>
         <v>0.346031746031746</v>
       </c>
       <c r="N3" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="R3" s="0" t="n">
+      <c r="R3" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="S3" s="0" t="n">
+      <c r="S3" s="1" t="n">
         <v>30</v>
       </c>
-      <c r="T3" s="0" t="n">
+      <c r="T3" s="1" t="n">
         <v>49</v>
       </c>
-      <c r="U3" s="0" t="n">
+      <c r="U3" s="1" t="n">
         <v>322</v>
       </c>
-      <c r="V3" s="0" t="n">
+      <c r="V3" s="1" t="n">
         <f aca="false">45+86+6</f>
         <v>137</v>
       </c>
-      <c r="W3" s="0" t="n">
+      <c r="W3" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="X3" s="0" t="n">
+      <c r="X3" s="1" t="n">
         <v>23</v>
       </c>
-      <c r="Y3" s="0" t="n">
+      <c r="Y3" s="1" t="n">
         <v>484</v>
       </c>
-      <c r="Z3" s="0" t="n">
+      <c r="Z3" s="1" t="n">
         <v>16</v>
       </c>
-      <c r="AA3" s="0" t="n">
+      <c r="AA3" s="1" t="n">
         <f aca="false">54+443+178</f>
         <v>675</v>
       </c>
-      <c r="AB3" s="0" t="n">
+      <c r="AB3" s="1" t="n">
         <v>232</v>
       </c>
-      <c r="AC3" s="0" t="n">
+      <c r="AC3" s="1" t="n">
         <v>36</v>
       </c>
-      <c r="AD3" s="0" t="n">
+      <c r="AD3" s="1" t="n">
         <v>959</v>
       </c>
-      <c r="AE3" s="0" t="s">
+      <c r="AE3" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="AF3" s="0" t="s">
+      <c r="AF3" s="1" t="s">
         <v>56</v>
       </c>
       <c r="AH3" s="2" t="n">
@@ -951,7 +953,7 @@
         <f aca="false">(V3+AA3)/(Y3+AD3)</f>
         <v>0.562716562716563</v>
       </c>
-      <c r="AP3" s="0" t="s">
+      <c r="AP3" s="1" t="s">
         <v>47</v>
       </c>
     </row>
@@ -959,88 +961,88 @@
       <c r="A4" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B4" s="0" t="n">
+      <c r="B4" s="1" t="n">
         <v>2024</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="F4" s="0" t="s">
+      <c r="F4" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="G4" s="0" t="s">
+      <c r="G4" s="1" t="s">
         <v>46</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>47</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J4" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="K4" s="0" t="s">
+      <c r="K4" s="1" t="s">
         <v>49</v>
       </c>
       <c r="L4" s="1" t="n">
         <f aca="false">28/(49+28)</f>
         <v>0.363636363636364</v>
       </c>
-      <c r="M4" s="0" t="n">
+      <c r="M4" s="1" t="n">
         <f aca="false">1-(1443+1441)/(49*90)</f>
         <v>0.346031746031746</v>
       </c>
       <c r="N4" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="R4" s="0" t="n">
+      <c r="R4" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="S4" s="0" t="n">
+      <c r="S4" s="1" t="n">
         <v>30</v>
       </c>
-      <c r="T4" s="0" t="n">
+      <c r="T4" s="1" t="n">
         <v>49</v>
       </c>
-      <c r="U4" s="0" t="n">
+      <c r="U4" s="1" t="n">
         <v>254</v>
       </c>
-      <c r="V4" s="0" t="n">
+      <c r="V4" s="1" t="n">
         <f aca="false">41+138+24</f>
         <v>203</v>
       </c>
-      <c r="W4" s="0" t="n">
+      <c r="W4" s="1" t="n">
         <v>16</v>
       </c>
-      <c r="X4" s="0" t="n">
+      <c r="X4" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="Y4" s="0" t="n">
+      <c r="Y4" s="1" t="n">
         <f aca="false">SUM(U4:X4)</f>
         <v>483</v>
       </c>
-      <c r="Z4" s="0" t="n">
+      <c r="Z4" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="AA4" s="0" t="n">
+      <c r="AA4" s="1" t="n">
         <f aca="false">48+414+139</f>
         <v>601</v>
       </c>
-      <c r="AB4" s="0" t="n">
+      <c r="AB4" s="1" t="n">
         <v>318</v>
       </c>
-      <c r="AC4" s="0" t="n">
+      <c r="AC4" s="1" t="n">
         <v>29</v>
       </c>
-      <c r="AD4" s="0" t="n">
+      <c r="AD4" s="1" t="n">
         <f aca="false">SUM(Z4:AC4)</f>
         <v>958</v>
       </c>
-      <c r="AE4" s="0" t="s">
+      <c r="AE4" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="AF4" s="0" t="s">
+      <c r="AF4" s="1" t="s">
         <v>56</v>
       </c>
       <c r="AH4" s="2" t="n">
@@ -1075,7 +1077,7 @@
         <f aca="false">(V4+AA4)/(Y4+AD4)</f>
         <v>0.55794587092297</v>
       </c>
-      <c r="AP4" s="0" t="s">
+      <c r="AP4" s="1" t="s">
         <v>47</v>
       </c>
     </row>
@@ -1195,9 +1197,6 @@
       <c r="AP5" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="AQ5" s="0"/>
-      <c r="AR5" s="0"/>
-      <c r="AS5" s="0"/>
     </row>
     <row r="6" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
@@ -1315,9 +1314,6 @@
       <c r="AP6" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="AQ6" s="0"/>
-      <c r="AR6" s="0"/>
-      <c r="AS6" s="0"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
@@ -2526,9 +2522,9 @@
       <c r="N17" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="O17" s="0"/>
-      <c r="P17" s="0"/>
-      <c r="Q17" s="0"/>
+      <c r="O17" s="1"/>
+      <c r="P17" s="1"/>
+      <c r="Q17" s="1"/>
       <c r="R17" s="1" t="n">
         <v>10</v>
       </c>
@@ -2606,9 +2602,9 @@
       <c r="AP17" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="AQ17" s="0"/>
-      <c r="AR17" s="0"/>
-      <c r="AS17" s="0"/>
+      <c r="AQ17" s="1"/>
+      <c r="AR17" s="1"/>
+      <c r="AS17" s="1"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
@@ -3233,9 +3229,9 @@
       <c r="P23" s="1" t="n">
         <v>124</v>
       </c>
-      <c r="Q23" s="0"/>
-      <c r="R23" s="0"/>
-      <c r="S23" s="0"/>
+      <c r="Q23" s="1"/>
+      <c r="R23" s="1"/>
+      <c r="S23" s="1"/>
       <c r="T23" s="1" t="n">
         <v>64</v>
       </c>
@@ -3307,9 +3303,9 @@
       <c r="AP23" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="AQ23" s="0"/>
-      <c r="AR23" s="0"/>
-      <c r="AS23" s="0"/>
+      <c r="AQ23" s="1"/>
+      <c r="AR23" s="1"/>
+      <c r="AS23" s="1"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="4" t="s">

</xml_diff>

<commit_message>
Updates -- grammarly and small fixes
</commit_message>
<xml_diff>
--- a/data/Study_Summary.xlsx
+++ b/data/Study_Summary.xlsx
@@ -347,7 +347,7 @@
     <t xml:space="preserve">stromanEmpiricallyDeterminedFrequency2014</t>
   </si>
   <si>
-    <t xml:space="preserve">fadulEmpiricalStudyImprove2013a</t>
+    <t xml:space="preserve">fadul</t>
   </si>
   <si>
     <t xml:space="preserve">Slide</t>
@@ -569,7 +569,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="P1" activeCellId="0" sqref="P1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M6" activeCellId="0" sqref="M6"/>
+      <selection pane="bottomRight" activeCell="A22" activeCellId="0" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -580,7 +580,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="9.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="5.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="21.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="18.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="18.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="7.93"/>
     <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="33" min="33" style="1" width="11.53"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="35" min="34" style="2" width="11.53"/>

</xml_diff>